<commit_message>
update harian tusbung sendiri
</commit_message>
<xml_diff>
--- a/17 nov Format Import Tusbung Harian.xlsx
+++ b/17 nov Format Import Tusbung Harian.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\billmanplnt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A493F3-4624-48FD-BCB8-B921B2272372}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9A244A3-3ECA-4507-A3AC-F39BC864323A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="1" xr2:uid="{AFDB4832-0DB3-4261-BED5-0029AE39DDBF}"/>
   </bookViews>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="179021"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -13348,7 +13348,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A83843FA-0508-4C7D-9F10-83AEAE723B47}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A83843FA-0508-4C7D-9F10-83AEAE723B47}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField numFmtId="1" showAll="0"/>
@@ -14296,8 +14296,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:P476"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A293" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="S315" sqref="S315"/>
+    <sheetView tabSelected="1" topLeftCell="A355" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="P254" sqref="P254:P476"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25826,7 +25826,7 @@
         <v>19961</v>
       </c>
       <c r="P254" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="255" spans="1:16" x14ac:dyDescent="0.25">
@@ -25872,7 +25872,7 @@
         <v>108629</v>
       </c>
       <c r="P255" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="256" spans="1:16" x14ac:dyDescent="0.25">
@@ -25918,7 +25918,7 @@
         <v>122905</v>
       </c>
       <c r="P256" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="257" spans="1:16" x14ac:dyDescent="0.25">
@@ -25964,7 +25964,7 @@
         <v>104163</v>
       </c>
       <c r="P257" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="258" spans="1:16" x14ac:dyDescent="0.25">
@@ -26010,7 +26010,7 @@
         <v>634723</v>
       </c>
       <c r="P258" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="259" spans="1:16" x14ac:dyDescent="0.25">
@@ -26056,7 +26056,7 @@
         <v>33171</v>
       </c>
       <c r="P259" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="260" spans="1:16" x14ac:dyDescent="0.25">
@@ -26102,7 +26102,7 @@
         <v>29092</v>
       </c>
       <c r="P260" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="261" spans="1:16" x14ac:dyDescent="0.25">
@@ -26148,7 +26148,7 @@
         <v>39799</v>
       </c>
       <c r="P261" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="262" spans="1:16" x14ac:dyDescent="0.25">
@@ -26194,7 +26194,7 @@
         <v>42081</v>
       </c>
       <c r="P262" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="263" spans="1:16" x14ac:dyDescent="0.25">
@@ -26240,7 +26240,7 @@
         <v>5099</v>
       </c>
       <c r="P263" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="264" spans="1:16" x14ac:dyDescent="0.25">
@@ -26286,7 +26286,7 @@
         <v>166577</v>
       </c>
       <c r="P264" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="265" spans="1:16" x14ac:dyDescent="0.25">
@@ -26332,7 +26332,7 @@
         <v>34701</v>
       </c>
       <c r="P265" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="266" spans="1:16" x14ac:dyDescent="0.25">
@@ -26378,7 +26378,7 @@
         <v>132082</v>
       </c>
       <c r="P266" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="267" spans="1:16" x14ac:dyDescent="0.25">
@@ -26424,7 +26424,7 @@
         <v>84666</v>
       </c>
       <c r="P267" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="268" spans="1:16" x14ac:dyDescent="0.25">
@@ -26516,7 +26516,7 @@
         <v>25014</v>
       </c>
       <c r="P269" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="270" spans="1:16" x14ac:dyDescent="0.25">
@@ -26608,7 +26608,7 @@
         <v>30622</v>
       </c>
       <c r="P271" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="272" spans="1:16" x14ac:dyDescent="0.25">
@@ -26700,7 +26700,7 @@
         <v>321417</v>
       </c>
       <c r="P273" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="274" spans="1:16" x14ac:dyDescent="0.25">
@@ -26746,7 +26746,7 @@
         <v>18849</v>
       </c>
       <c r="P274" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="275" spans="1:16" x14ac:dyDescent="0.25">
@@ -26792,7 +26792,7 @@
         <v>104442</v>
       </c>
       <c r="P275" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="276" spans="1:16" x14ac:dyDescent="0.25">
@@ -26884,7 +26884,7 @@
         <v>166242</v>
       </c>
       <c r="P277" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="278" spans="1:16" x14ac:dyDescent="0.25">
@@ -26976,7 +26976,7 @@
         <v>64272</v>
       </c>
       <c r="P279" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="280" spans="1:16" x14ac:dyDescent="0.25">
@@ -27114,7 +27114,7 @@
         <v>327096</v>
       </c>
       <c r="P282" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="283" spans="1:16" x14ac:dyDescent="0.25">
@@ -27160,7 +27160,7 @@
         <v>269040</v>
       </c>
       <c r="P283" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="284" spans="1:16" x14ac:dyDescent="0.25">
@@ -27252,7 +27252,7 @@
         <v>223020</v>
       </c>
       <c r="P285" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="286" spans="1:16" x14ac:dyDescent="0.25">
@@ -27298,7 +27298,7 @@
         <v>144900</v>
       </c>
       <c r="P286" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="287" spans="1:16" x14ac:dyDescent="0.25">
@@ -27344,7 +27344,7 @@
         <v>93746</v>
       </c>
       <c r="P287" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="288" spans="1:16" x14ac:dyDescent="0.25">
@@ -27390,7 +27390,7 @@
         <v>98942</v>
       </c>
       <c r="P288" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="289" spans="1:16" x14ac:dyDescent="0.25">
@@ -27436,7 +27436,7 @@
         <v>177459</v>
       </c>
       <c r="P289" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="290" spans="1:16" x14ac:dyDescent="0.25">
@@ -27482,7 +27482,7 @@
         <v>41839</v>
       </c>
       <c r="P290" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="291" spans="1:16" x14ac:dyDescent="0.25">
@@ -27666,7 +27666,7 @@
         <v>113918</v>
       </c>
       <c r="P294" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="295" spans="1:16" x14ac:dyDescent="0.25">
@@ -27712,7 +27712,7 @@
         <v>16253</v>
       </c>
       <c r="P295" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="296" spans="1:16" x14ac:dyDescent="0.25">
@@ -27758,7 +27758,7 @@
         <v>65292</v>
       </c>
       <c r="P296" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="297" spans="1:16" x14ac:dyDescent="0.25">
@@ -27804,7 +27804,7 @@
         <v>343738</v>
       </c>
       <c r="P297" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="298" spans="1:16" x14ac:dyDescent="0.25">
@@ -27850,7 +27850,7 @@
         <v>245527</v>
       </c>
       <c r="P298" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="299" spans="1:16" x14ac:dyDescent="0.25">
@@ -27896,7 +27896,7 @@
         <v>44898</v>
       </c>
       <c r="P299" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="300" spans="1:16" x14ac:dyDescent="0.25">
@@ -27942,7 +27942,7 @@
         <v>115257</v>
       </c>
       <c r="P300" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="301" spans="1:16" x14ac:dyDescent="0.25">
@@ -27988,7 +27988,7 @@
         <v>51525</v>
       </c>
       <c r="P301" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="302" spans="1:16" x14ac:dyDescent="0.25">
@@ -28034,7 +28034,7 @@
         <v>66821</v>
       </c>
       <c r="P302" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="303" spans="1:16" x14ac:dyDescent="0.25">
@@ -28126,7 +28126,7 @@
         <v>69371</v>
       </c>
       <c r="P304" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="305" spans="1:16" x14ac:dyDescent="0.25">
@@ -28172,7 +28172,7 @@
         <v>44388</v>
       </c>
       <c r="P305" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="306" spans="1:16" x14ac:dyDescent="0.25">
@@ -28218,7 +28218,7 @@
         <v>162196</v>
       </c>
       <c r="P306" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="307" spans="1:16" x14ac:dyDescent="0.25">
@@ -28402,7 +28402,7 @@
         <v>330345</v>
       </c>
       <c r="P310" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="311" spans="1:16" x14ac:dyDescent="0.25">
@@ -28494,7 +28494,7 @@
         <v>69628</v>
       </c>
       <c r="P312" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="313" spans="1:16" x14ac:dyDescent="0.25">
@@ -28540,7 +28540,7 @@
         <v>50132</v>
       </c>
       <c r="P313" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="314" spans="1:16" x14ac:dyDescent="0.25">
@@ -28586,7 +28586,7 @@
         <v>1059062</v>
       </c>
       <c r="P314" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="315" spans="1:16" x14ac:dyDescent="0.25">
@@ -28632,7 +28632,7 @@
         <v>50132</v>
       </c>
       <c r="P315" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="316" spans="1:16" x14ac:dyDescent="0.25">
@@ -28678,7 +28678,7 @@
         <v>12175</v>
       </c>
       <c r="P316" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="317" spans="1:16" x14ac:dyDescent="0.25">
@@ -28724,7 +28724,7 @@
         <v>49996</v>
       </c>
       <c r="P317" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="318" spans="1:16" x14ac:dyDescent="0.25">
@@ -28770,7 +28770,7 @@
         <v>272291</v>
       </c>
       <c r="P318" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="319" spans="1:16" x14ac:dyDescent="0.25">
@@ -28816,7 +28816,7 @@
         <v>147887</v>
       </c>
       <c r="P319" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="320" spans="1:16" x14ac:dyDescent="0.25">
@@ -28862,7 +28862,7 @@
         <v>148907</v>
       </c>
       <c r="P320" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="321" spans="1:16" x14ac:dyDescent="0.25">
@@ -28908,7 +28908,7 @@
         <v>215766</v>
       </c>
       <c r="P321" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="322" spans="1:16" x14ac:dyDescent="0.25">
@@ -28954,7 +28954,7 @@
         <v>354154</v>
       </c>
       <c r="P322" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="323" spans="1:16" x14ac:dyDescent="0.25">
@@ -29000,7 +29000,7 @@
         <v>35211</v>
       </c>
       <c r="P323" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="324" spans="1:16" x14ac:dyDescent="0.25">
@@ -29092,7 +29092,7 @@
         <v>96393</v>
       </c>
       <c r="P325" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="326" spans="1:16" x14ac:dyDescent="0.25">
@@ -29184,7 +29184,7 @@
         <v>77528</v>
       </c>
       <c r="P327" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="328" spans="1:16" x14ac:dyDescent="0.25">
@@ -29230,7 +29230,7 @@
         <v>65450</v>
       </c>
       <c r="P328" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="329" spans="1:16" x14ac:dyDescent="0.25">
@@ -29276,7 +29276,7 @@
         <v>77378</v>
       </c>
       <c r="P329" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="330" spans="1:16" x14ac:dyDescent="0.25">
@@ -29322,7 +29322,7 @@
         <v>6839</v>
       </c>
       <c r="P330" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="331" spans="1:16" x14ac:dyDescent="0.25">
@@ -29368,7 +29368,7 @@
         <v>396000</v>
       </c>
       <c r="P331" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="332" spans="1:16" x14ac:dyDescent="0.25">
@@ -29460,7 +29460,7 @@
         <v>419161</v>
       </c>
       <c r="P333" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="334" spans="1:16" x14ac:dyDescent="0.25">
@@ -29506,7 +29506,7 @@
         <v>31642</v>
       </c>
       <c r="P334" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="335" spans="1:16" x14ac:dyDescent="0.25">
@@ -29552,7 +29552,7 @@
         <v>372010</v>
       </c>
       <c r="P335" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="336" spans="1:16" x14ac:dyDescent="0.25">
@@ -29598,7 +29598,7 @@
         <v>55605</v>
       </c>
       <c r="P336" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="337" spans="1:16" x14ac:dyDescent="0.25">
@@ -29644,7 +29644,7 @@
         <v>83646</v>
       </c>
       <c r="P337" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="338" spans="1:16" x14ac:dyDescent="0.25">
@@ -29690,7 +29690,7 @@
         <v>84156</v>
       </c>
       <c r="P338" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="339" spans="1:16" x14ac:dyDescent="0.25">
@@ -29736,7 +29736,7 @@
         <v>47957</v>
       </c>
       <c r="P339" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="340" spans="1:16" x14ac:dyDescent="0.25">
@@ -29782,7 +29782,7 @@
         <v>77528</v>
       </c>
       <c r="P340" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="341" spans="1:16" x14ac:dyDescent="0.25">
@@ -29828,7 +29828,7 @@
         <v>21074</v>
       </c>
       <c r="P341" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="342" spans="1:16" x14ac:dyDescent="0.25">
@@ -29920,7 +29920,7 @@
         <v>90784</v>
       </c>
       <c r="P343" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="344" spans="1:16" x14ac:dyDescent="0.25">
@@ -30012,7 +30012,7 @@
         <v>47447</v>
       </c>
       <c r="P345" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="346" spans="1:16" x14ac:dyDescent="0.25">
@@ -30058,7 +30058,7 @@
         <v>47957</v>
       </c>
       <c r="P346" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="347" spans="1:16" x14ac:dyDescent="0.25">
@@ -30104,7 +30104,7 @@
         <v>26033</v>
       </c>
       <c r="P347" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="348" spans="1:16" x14ac:dyDescent="0.25">
@@ -30150,7 +30150,7 @@
         <v>55095</v>
       </c>
       <c r="P348" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="349" spans="1:16" x14ac:dyDescent="0.25">
@@ -30196,7 +30196,7 @@
         <v>71920</v>
       </c>
       <c r="P349" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="350" spans="1:16" x14ac:dyDescent="0.25">
@@ -30242,7 +30242,7 @@
         <v>49996</v>
       </c>
       <c r="P350" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="351" spans="1:16" x14ac:dyDescent="0.25">
@@ -30288,7 +30288,7 @@
         <v>97412</v>
       </c>
       <c r="P351" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="352" spans="1:16" x14ac:dyDescent="0.25">
@@ -30334,7 +30334,7 @@
         <v>229973</v>
       </c>
       <c r="P352" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="353" spans="1:16" x14ac:dyDescent="0.25">
@@ -30426,7 +30426,7 @@
         <v>794614</v>
       </c>
       <c r="P354" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="355" spans="1:16" x14ac:dyDescent="0.25">
@@ -30472,7 +30472,7 @@
         <v>42348</v>
       </c>
       <c r="P355" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="356" spans="1:16" x14ac:dyDescent="0.25">
@@ -30518,7 +30518,7 @@
         <v>251479</v>
       </c>
       <c r="P356" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="357" spans="1:16" x14ac:dyDescent="0.25">
@@ -30564,7 +30564,7 @@
         <v>36740</v>
       </c>
       <c r="P357" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="358" spans="1:16" x14ac:dyDescent="0.25">
@@ -30610,7 +30610,7 @@
         <v>22974</v>
       </c>
       <c r="P358" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="359" spans="1:16" x14ac:dyDescent="0.25">
@@ -30656,7 +30656,7 @@
         <v>90274</v>
       </c>
       <c r="P359" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="360" spans="1:16" x14ac:dyDescent="0.25">
@@ -30702,7 +30702,7 @@
         <v>163685</v>
       </c>
       <c r="P360" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="361" spans="1:16" x14ac:dyDescent="0.25">
@@ -30748,7 +30748,7 @@
         <v>111688</v>
       </c>
       <c r="P361" s="15" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="362" spans="1:16" hidden="1" x14ac:dyDescent="0.25">

</xml_diff>